<commit_message>
potok magic calculator, test fix for short execution
</commit_message>
<xml_diff>
--- a/potok/MAGIC_CALCULATOR.xlsx
+++ b/potok/MAGIC_CALCULATOR.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="28">
   <si>
     <t>buy</t>
   </si>
@@ -92,6 +92,18 @@
   </si>
   <si>
     <t>CLOSE_SHORT</t>
+  </si>
+  <si>
+    <t>BUY ORDER SAMPLE</t>
+  </si>
+  <si>
+    <t>SELL ORDER SAMPLE</t>
+  </si>
+  <si>
+    <t>SHORT ORDER SAMPLE</t>
+  </si>
+  <si>
+    <t>CLOSE_SHORT SAMPLE</t>
   </si>
 </sst>
 </file>
@@ -135,10 +147,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -531,13 +546,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W17"/>
+  <dimension ref="A1:W40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
+      <selection pane="bottomRight" activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,21 +811,21 @@
         <v>9</v>
       </c>
       <c r="D8">
-        <f>(C$6-C8)*C7</f>
+        <f>(C6-C8)*C7</f>
         <v>50</v>
       </c>
       <c r="E8">
         <v>9</v>
       </c>
       <c r="F8">
-        <f>(E$6-E8)*E7</f>
+        <f>(E6-E8)*E7</f>
         <v>10</v>
       </c>
       <c r="G8">
         <v>8</v>
       </c>
       <c r="H8">
-        <f>(G$6-G8)*G7</f>
+        <f>(G6-G8)*G7</f>
         <v>180</v>
       </c>
       <c r="I8">
@@ -859,7 +874,7 @@
         <v>9</v>
       </c>
       <c r="V8">
-        <f>(U$6-U8)*U7</f>
+        <f>(U6-U8)*U7</f>
         <v>180</v>
       </c>
     </row>
@@ -906,21 +921,21 @@
         <v>10</v>
       </c>
       <c r="D10">
-        <f>(C$6-C10)*C9</f>
+        <f>(C6-C10)*C9</f>
         <v>0</v>
       </c>
       <c r="E10">
         <v>10</v>
       </c>
       <c r="F10">
-        <f>(E$6-E10)*E9</f>
+        <f>(E6-E10)*E9</f>
         <v>0</v>
       </c>
       <c r="G10">
         <v>9</v>
       </c>
       <c r="H10">
-        <f>(G$6-G10)*G9</f>
+        <f>(G6-G10)*G9</f>
         <v>10</v>
       </c>
       <c r="I10">
@@ -969,7 +984,7 @@
         <v>0</v>
       </c>
       <c r="V10">
-        <f>(U$6-U10)*U9</f>
+        <f>(U6-U10)*U9</f>
         <v>0</v>
       </c>
     </row>
@@ -1190,11 +1205,11 @@
         <v>-1620</v>
       </c>
       <c r="W16">
-        <f>W15*E1</f>
+        <f>W15*$E$1</f>
         <v>2160</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1203,7 +1218,266 @@
         <v>999930</v>
       </c>
     </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J26" s="2"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29">
+        <v>120</v>
+      </c>
+      <c r="E29">
+        <v>-100</v>
+      </c>
+      <c r="G29">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30">
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <f>-(C29*C30)</f>
+        <v>-1200</v>
+      </c>
+      <c r="E30">
+        <v>10</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>11</v>
+      </c>
+      <c r="H30">
+        <f>$E$1*G29</f>
+        <v>-1200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31">
+        <v>100</v>
+      </c>
+      <c r="E31">
+        <v>50</v>
+      </c>
+      <c r="G31">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32">
+        <v>9</v>
+      </c>
+      <c r="D32">
+        <f>(C30-C32)*C31</f>
+        <v>100</v>
+      </c>
+      <c r="E32">
+        <v>11</v>
+      </c>
+      <c r="F32">
+        <f>E32*E31</f>
+        <v>550</v>
+      </c>
+      <c r="G32">
+        <v>11</v>
+      </c>
+      <c r="H32">
+        <f>G32*G31</f>
+        <v>550</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33">
+        <v>20</v>
+      </c>
+      <c r="E33">
+        <v>10</v>
+      </c>
+      <c r="G33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34">
+        <v>10</v>
+      </c>
+      <c r="D34">
+        <f>(C30-C34)*C33</f>
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>10</v>
+      </c>
+      <c r="F34">
+        <f>E34*E33</f>
+        <v>100</v>
+      </c>
+      <c r="G34">
+        <v>12</v>
+      </c>
+      <c r="H34">
+        <f>G34*G33</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <f>C35*C30</f>
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36">
+        <f>ABS(C29)-C31-C33-C35</f>
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <f>ABS(E29)-E31-E33-E35</f>
+        <v>40</v>
+      </c>
+      <c r="G36">
+        <f>ABS(G29)-G31-G33-G35</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38">
+        <f>SUM(C38:QT38)</f>
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <f>C31+C33</f>
+        <v>120</v>
+      </c>
+      <c r="E38">
+        <f>-(E31+E33)</f>
+        <v>-60</v>
+      </c>
+      <c r="I38">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39">
+        <f>SUM(C39:QT39)</f>
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <f>-(G31+G33)</f>
+        <v>-60</v>
+      </c>
+      <c r="I39">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40">
+        <f>SUM(C40:CF40)</f>
+        <v>-260</v>
+      </c>
+      <c r="D40">
+        <f>SUM(D29:D39)</f>
+        <v>-1100</v>
+      </c>
+      <c r="F40">
+        <f>SUM(F29:F39)</f>
+        <v>650</v>
+      </c>
+      <c r="H40">
+        <f>SUM(H29:H39)</f>
+        <v>-530</v>
+      </c>
+      <c r="I40">
+        <f>I39*$E$1</f>
+        <v>720</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>